<commit_message>
fix hannover 2015 date format
</commit_message>
<xml_diff>
--- a/data/management/Management_information_HAN_2015.xlsx
+++ b/data/management/Management_information_HAN_2015.xlsx
@@ -1,18 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marse\seadrive_root\Tien-Che\My Libraries\PhD_Tien\Project\Briwecs\BRIWECS_Data_Publication\data\management\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6942C6-ECD2-4621-86E2-ABE105CDF13D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Tabelle2" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="Tabelle3" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
+    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -24,345 +29,343 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="109">
   <si>
-    <t xml:space="preserve">General information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Farm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Versuchsstation IGPS Ruthe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postal code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31157</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schäferberg 9, 31157 Sarstedt OT Ruthe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Federal state</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Niedersachsen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weather station</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IGPS and IMUK, both in Ruthe at the research station</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Distance from the closest weather station</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0 km</t>
+    <t>General information</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Farm</t>
+  </si>
+  <si>
+    <t>Versuchsstation IGPS Ruthe</t>
+  </si>
+  <si>
+    <t>Postal code</t>
+  </si>
+  <si>
+    <t>31157</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Schäferberg 9, 31157 Sarstedt OT Ruthe</t>
+  </si>
+  <si>
+    <t>Federal state</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Weather station</t>
+  </si>
+  <si>
+    <t>IGPS and IMUK, both in Ruthe at the research station</t>
+  </si>
+  <si>
+    <t>Distance from the closest weather station</t>
+  </si>
+  <si>
+    <t>0 km</t>
   </si>
   <si>
     <t xml:space="preserve">Correspondence </t>
   </si>
   <si>
-    <t xml:space="preserve">Carolin Lichthardt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intern ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plot information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plot length</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plot width</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plot size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12 m2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">harvest size of the plot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soil Condition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date of data collection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type of soil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clayey silt (toniger Schluff)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grade of soil productivity (Ackerzahl)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soil structure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sowing preperation (Saatbettbereitung)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maisstoppelbearbeitung, Pflug, Saatbettkombination</t>
-  </si>
-  <si>
-    <t xml:space="preserve">october 2014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Preceding crop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mais</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pre-Preceding crop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zuckerrüben</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soil cultivation before preceding crop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Catch crop (Zwischenfrucht)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">non</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clay</t>
+    <t>Carolin Lichthardt</t>
+  </si>
+  <si>
+    <t>Intern ID</t>
+  </si>
+  <si>
+    <t>Plot information</t>
+  </si>
+  <si>
+    <t>plot length</t>
+  </si>
+  <si>
+    <t>6 m</t>
+  </si>
+  <si>
+    <t>plot width</t>
+  </si>
+  <si>
+    <t>2 m</t>
+  </si>
+  <si>
+    <t>plot size</t>
+  </si>
+  <si>
+    <t>12 m2</t>
+  </si>
+  <si>
+    <t>harvest size of the plot</t>
+  </si>
+  <si>
+    <t>Soil Condition</t>
+  </si>
+  <si>
+    <t>Date of data collection</t>
+  </si>
+  <si>
+    <t>Type of soil</t>
+  </si>
+  <si>
+    <t>clayey silt (toniger Schluff)</t>
+  </si>
+  <si>
+    <t>Grade of soil productivity (Ackerzahl)</t>
+  </si>
+  <si>
+    <t>Soil structure</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Sowing preperation (Saatbettbereitung)</t>
+  </si>
+  <si>
+    <t>Maisstoppelbearbeitung, Pflug, Saatbettkombination</t>
+  </si>
+  <si>
+    <t>october 2014</t>
+  </si>
+  <si>
+    <t>Preceding crop</t>
+  </si>
+  <si>
+    <t>Mais</t>
+  </si>
+  <si>
+    <t>Pre-Preceding crop</t>
+  </si>
+  <si>
+    <t>Zuckerrüben</t>
+  </si>
+  <si>
+    <t>Soil cultivation before preceding crop</t>
+  </si>
+  <si>
+    <t>Catch crop (Zwischenfrucht)</t>
+  </si>
+  <si>
+    <t>non</t>
+  </si>
+  <si>
+    <t>Clay</t>
   </si>
   <si>
     <t xml:space="preserve">Sand </t>
   </si>
   <si>
-    <t xml:space="preserve">Silt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">organical content</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P2O5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33 (mg/100g)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K2O</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11 (mg/100g)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C/N ratio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nicht ermittelt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soil nitrogen, 0-30cm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soil nitrogen, 30-60cm</t>
+    <t>Silt</t>
+  </si>
+  <si>
+    <t>pH</t>
+  </si>
+  <si>
+    <t>organical content</t>
+  </si>
+  <si>
+    <t>P2O5</t>
+  </si>
+  <si>
+    <t>33 (mg/100g)</t>
+  </si>
+  <si>
+    <t>K2O</t>
+  </si>
+  <si>
+    <t>11 (mg/100g)</t>
+  </si>
+  <si>
+    <t>C/N ratio</t>
+  </si>
+  <si>
+    <t>nicht ermittelt</t>
+  </si>
+  <si>
+    <t>Soil nitrogen, 0-30cm</t>
+  </si>
+  <si>
+    <t>Soil nitrogen, 30-60cm</t>
   </si>
   <si>
     <t xml:space="preserve">Soil nitrogen, 60-90cm </t>
   </si>
   <si>
-    <t xml:space="preserve">Soil nitrogen, 0-90cm</t>
+    <t>Soil nitrogen, 0-90cm</t>
   </si>
   <si>
     <t xml:space="preserve">Available nitrogen in fine soil </t>
   </si>
   <si>
-    <t xml:space="preserve">Managements</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Treatment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fertilization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date (dd.mm.YYYY)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plant protection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Infection_data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Measure Date (dd.mm.YYYY)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">low nitrogen, no fungicide (LN_NF)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1st nitrogen application</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eigntl.40kg/ha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1st herbicide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,2l/ha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Axial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stripe_rust</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.06.2015 - 19.06.2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2nd nitrogen application</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2nd herbicide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">70g+1l+20g/ha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biathlon4D+Dash+Dirigent SX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Powdery_mildew</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3rd nitrogen application</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1st application of insecticide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,2l/ha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sumicidien</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leaf_rust</t>
-  </si>
-  <si>
-    <t xml:space="preserve">others</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2nd application of insecticide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Septoria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1st application of fungicide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DTR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2nd application of fungicide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fusarium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3rd application of fungicide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1st application of growth regulator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2nd application of growth regulator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">high nitrogen, no fungicide (HN_NF)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eigntl.50kg/ha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,2 l/ha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stabilon 720</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,5 l/ha+0,5 l/ha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stabilon720+Medox Top</t>
-  </si>
-  <si>
-    <t xml:space="preserve">high nitrogen, with fungicide (HN_WF)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2l/ha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capalo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,1l/ha+1,1l/ha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adexa+Diamant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16-062015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1l/ha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prosaro</t>
+    <t>Managements</t>
+  </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>Fertilization</t>
+  </si>
+  <si>
+    <t>Date (dd.mm.YYYY)</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Notice</t>
+  </si>
+  <si>
+    <t>Plant protection</t>
+  </si>
+  <si>
+    <t>Infection_data</t>
+  </si>
+  <si>
+    <t>Measure Date (dd.mm.YYYY)</t>
+  </si>
+  <si>
+    <t>low nitrogen, no fungicide (LN_NF)</t>
+  </si>
+  <si>
+    <t>1st nitrogen application</t>
+  </si>
+  <si>
+    <t>eigntl.40kg/ha</t>
+  </si>
+  <si>
+    <t>1st herbicide</t>
+  </si>
+  <si>
+    <t>1,2l/ha</t>
+  </si>
+  <si>
+    <t>Axial</t>
+  </si>
+  <si>
+    <t>Stripe_rust</t>
+  </si>
+  <si>
+    <t>8.06.2015 - 19.06.2015</t>
+  </si>
+  <si>
+    <t>2nd nitrogen application</t>
+  </si>
+  <si>
+    <t>2nd herbicide</t>
+  </si>
+  <si>
+    <t>70g+1l+20g/ha</t>
+  </si>
+  <si>
+    <t>Biathlon4D+Dash+Dirigent SX</t>
+  </si>
+  <si>
+    <t>Powdery_mildew</t>
+  </si>
+  <si>
+    <t>3rd nitrogen application</t>
+  </si>
+  <si>
+    <t>1st application of insecticide</t>
+  </si>
+  <si>
+    <t>0,2l/ha</t>
+  </si>
+  <si>
+    <t>Sumicidien</t>
+  </si>
+  <si>
+    <t>Leaf_rust</t>
+  </si>
+  <si>
+    <t>others</t>
+  </si>
+  <si>
+    <t>2nd application of insecticide</t>
+  </si>
+  <si>
+    <t>Septoria</t>
+  </si>
+  <si>
+    <t>1st application of fungicide</t>
+  </si>
+  <si>
+    <t>DTR</t>
+  </si>
+  <si>
+    <t>2nd application of fungicide</t>
+  </si>
+  <si>
+    <t>Fusarium</t>
+  </si>
+  <si>
+    <t>3rd application of fungicide</t>
+  </si>
+  <si>
+    <t>1st application of growth regulator</t>
+  </si>
+  <si>
+    <t>2nd application of growth regulator</t>
+  </si>
+  <si>
+    <t>high nitrogen, no fungicide (HN_NF)</t>
+  </si>
+  <si>
+    <t>eigntl.50kg/ha</t>
+  </si>
+  <si>
+    <t>1,2 l/ha</t>
+  </si>
+  <si>
+    <t>Stabilon 720</t>
+  </si>
+  <si>
+    <t>0,5 l/ha+0,5 l/ha</t>
+  </si>
+  <si>
+    <t>Stabilon720+Medox Top</t>
+  </si>
+  <si>
+    <t>high nitrogen, with fungicide (HN_WF)</t>
+  </si>
+  <si>
+    <t>2l/ha</t>
+  </si>
+  <si>
+    <t>Capalo</t>
+  </si>
+  <si>
+    <t>1,1l/ha+1,1l/ha</t>
+  </si>
+  <si>
+    <t>Adexa+Diamant</t>
+  </si>
+  <si>
+    <t>1l/ha</t>
+  </si>
+  <si>
+    <t>Prosaro</t>
+  </si>
+  <si>
+    <t>16/06/2015</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="0.00\ %"/>
-    <numFmt numFmtId="167" formatCode="mmm\ yy"/>
-    <numFmt numFmtId="168" formatCode="dd/mm/yyyy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="0.00\ %"/>
+    <numFmt numFmtId="165" formatCode="mmm\ yy"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -371,22 +374,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -394,7 +382,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
@@ -402,7 +390,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -410,7 +398,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -420,6 +408,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -446,7 +441,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.7999"/>
+        <fgColor theme="6" tint="0.79989013336588644"/>
         <bgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
@@ -458,38 +453,38 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.3999"/>
+        <fgColor theme="3" tint="0.39988402966399123"/>
         <bgColor rgb="FF7F7F7F"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.5999"/>
+        <fgColor theme="4" tint="0.59987182226020086"/>
         <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.7999"/>
+        <fgColor theme="7" tint="0.79989013336588644"/>
         <bgColor rgb="FFEBF1DE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.7999"/>
+        <fgColor theme="9" tint="0.79989013336588644"/>
         <bgColor rgb="FFEBF1DE"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="5">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -504,7 +499,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -519,7 +514,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -532,129 +527,63 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="2" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="3" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="4" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="4">
+    <cellStyle name="Excel Built-in 20% - Accent3" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Excel Built-in Input" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Excel Built-in Output" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Excel Built-in Output" xfId="20"/>
-    <cellStyle name="Excel Built-in Input" xfId="21"/>
-    <cellStyle name="Excel Built-in 20% - Accent3" xfId="22"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -713,47 +642,63 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF3F3F76"/>
       <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1f497d"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="eeece1"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4f81bd"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="c0504d"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9bbb59"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064a2"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4bacc6"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="f79646"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000ff"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
         <a:srgbClr val="800080"/>
@@ -761,12 +706,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -795,7 +740,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="1"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -816,7 +761,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -867,7 +812,7 @@
           <a:path path="circle">
             <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -885,51 +830,50 @@
           <a:path path="circle">
             <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B37" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="C40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="33.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="36.54"/>
+    <col min="1" max="1" width="43.140625" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
+    <col min="6" max="6" width="33.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" customWidth="1"/>
+    <col min="11" max="11" width="36.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="2">
         <v>2014</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -937,7 +881,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -945,7 +889,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -953,7 +897,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -961,7 +905,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -969,7 +913,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -977,7 +921,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -985,19 +929,19 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="2"/>
     </row>
-    <row r="12" customFormat="false" ht="45.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:2" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -1005,7 +949,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -1013,7 +957,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -1021,7 +965,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
@@ -1029,21 +973,21 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:3" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>27</v>
       </c>
@@ -1052,16 +996,16 @@
       </c>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="6" t="n">
+      <c r="B21" s="6">
         <v>80</v>
       </c>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>30</v>
       </c>
@@ -1070,7 +1014,7 @@
       </c>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>32</v>
       </c>
@@ -1081,7 +1025,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>35</v>
       </c>
@@ -1090,7 +1034,7 @@
       </c>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>37</v>
       </c>
@@ -1099,7 +1043,7 @@
       </c>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>39</v>
       </c>
@@ -1108,7 +1052,7 @@
       </c>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>40</v>
       </c>
@@ -1117,52 +1061,52 @@
       </c>
       <c r="C27" s="2"/>
     </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="7" t="n">
-        <v>0.137</v>
+      <c r="B28" s="7">
+        <v>0.13700000000000001</v>
       </c>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="7" t="n">
-        <v>0.075</v>
+      <c r="B29" s="7">
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="C29" s="2"/>
     </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="7" t="n">
-        <v>0.788</v>
+      <c r="B30" s="7">
+        <v>0.78800000000000003</v>
       </c>
       <c r="C30" s="2"/>
     </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B31" s="6" t="n">
+      <c r="B31" s="6">
         <v>7.1</v>
       </c>
       <c r="C31" s="2"/>
     </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="7" t="n">
-        <v>0.0295</v>
+      <c r="B32" s="7">
+        <v>2.9499999999999998E-2</v>
       </c>
       <c r="C32" s="2"/>
     </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>47</v>
       </c>
@@ -1171,7 +1115,7 @@
       </c>
       <c r="C33" s="2"/>
     </row>
-    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>49</v>
       </c>
@@ -1180,7 +1124,7 @@
       </c>
       <c r="C34" s="2"/>
     </row>
-    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>51</v>
       </c>
@@ -1189,51 +1133,51 @@
       </c>
       <c r="C35" s="2"/>
     </row>
-    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B36" s="6" t="n">
+      <c r="B36" s="6">
         <v>10.9</v>
       </c>
-      <c r="C36" s="8" t="n">
+      <c r="C36" s="8">
         <v>42095</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B37" s="6" t="n">
-        <v>16.6</v>
-      </c>
-      <c r="C37" s="8" t="n">
+      <c r="B37" s="6">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="C37" s="8">
         <v>42095</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B38" s="6" t="n">
+      <c r="B38" s="6">
         <v>43.2</v>
       </c>
-      <c r="C38" s="8" t="n">
+      <c r="C38" s="8">
         <v>42095</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B39" s="6" t="n">
+      <c r="B39" s="6">
         <v>70.7</v>
       </c>
-      <c r="C39" s="8" t="n">
+      <c r="C39" s="8">
         <v>42095</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>57</v>
       </c>
@@ -1242,7 +1186,7 @@
       </c>
       <c r="C40" s="2"/>
     </row>
-    <row r="42" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>58</v>
       </c>
@@ -1257,7 +1201,7 @@
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>59</v>
       </c>
@@ -1292,17 +1236,17 @@
         <v>66</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>67</v>
       </c>
       <c r="B44" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C44" s="12" t="n">
+      <c r="C44" s="12">
         <v>42076</v>
       </c>
-      <c r="D44" s="11" t="n">
+      <c r="D44" s="11">
         <v>0</v>
       </c>
       <c r="E44" s="11" t="s">
@@ -1311,7 +1255,7 @@
       <c r="F44" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="G44" s="14" t="n">
+      <c r="G44" s="14">
         <v>42082</v>
       </c>
       <c r="H44" s="13" t="s">
@@ -1327,24 +1271,24 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>67</v>
       </c>
       <c r="B45" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C45" s="12" t="n">
+      <c r="C45" s="12">
         <v>42129</v>
       </c>
-      <c r="D45" s="11" t="n">
+      <c r="D45" s="11">
         <v>0</v>
       </c>
       <c r="E45" s="11"/>
       <c r="F45" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="G45" s="14" t="n">
+      <c r="G45" s="14">
         <v>42087</v>
       </c>
       <c r="H45" s="13" t="s">
@@ -1358,24 +1302,24 @@
       </c>
       <c r="K45" s="15"/>
     </row>
-    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>67</v>
       </c>
       <c r="B46" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C46" s="12" t="n">
+      <c r="C46" s="12">
         <v>42151</v>
       </c>
-      <c r="D46" s="11" t="n">
+      <c r="D46" s="11">
         <v>0</v>
       </c>
       <c r="E46" s="11"/>
       <c r="F46" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="G46" s="14" t="n">
+      <c r="G46" s="14">
         <v>42159</v>
       </c>
       <c r="H46" s="13" t="s">
@@ -1389,8 +1333,8 @@
       </c>
       <c r="K46" s="15"/>
     </row>
-    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>67</v>
       </c>
       <c r="B47" s="11" t="s">
@@ -1402,13 +1346,13 @@
       <c r="F47" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="G47" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H47" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I47" s="13" t="n">
+      <c r="G47" s="13">
+        <v>0</v>
+      </c>
+      <c r="H47" s="13">
+        <v>0</v>
+      </c>
+      <c r="I47" s="13">
         <v>0</v>
       </c>
       <c r="J47" s="15" t="s">
@@ -1416,8 +1360,8 @@
       </c>
       <c r="K47" s="15"/>
     </row>
-    <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>67</v>
       </c>
       <c r="B48" s="11"/>
@@ -1427,13 +1371,13 @@
       <c r="F48" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="G48" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H48" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I48" s="13" t="n">
+      <c r="G48" s="13">
+        <v>0</v>
+      </c>
+      <c r="H48" s="13">
+        <v>0</v>
+      </c>
+      <c r="I48" s="13">
         <v>0</v>
       </c>
       <c r="J48" s="15" t="s">
@@ -1441,8 +1385,8 @@
       </c>
       <c r="K48" s="15"/>
     </row>
-    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>67</v>
       </c>
       <c r="B49" s="11"/>
@@ -1452,13 +1396,13 @@
       <c r="F49" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="G49" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H49" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I49" s="13" t="n">
+      <c r="G49" s="13">
+        <v>0</v>
+      </c>
+      <c r="H49" s="13">
+        <v>0</v>
+      </c>
+      <c r="I49" s="13">
         <v>0</v>
       </c>
       <c r="J49" s="15" t="s">
@@ -1466,8 +1410,8 @@
       </c>
       <c r="K49" s="15"/>
     </row>
-    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>67</v>
       </c>
       <c r="B50" s="11"/>
@@ -1477,20 +1421,20 @@
       <c r="F50" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="G50" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H50" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I50" s="13" t="n">
+      <c r="G50" s="13">
+        <v>0</v>
+      </c>
+      <c r="H50" s="13">
+        <v>0</v>
+      </c>
+      <c r="I50" s="13">
         <v>0</v>
       </c>
       <c r="J50" s="15"/>
       <c r="K50" s="15"/>
     </row>
-    <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>67</v>
       </c>
       <c r="B51" s="11"/>
@@ -1500,20 +1444,20 @@
       <c r="F51" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="G51" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H51" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I51" s="13" t="n">
+      <c r="G51" s="13">
+        <v>0</v>
+      </c>
+      <c r="H51" s="13">
+        <v>0</v>
+      </c>
+      <c r="I51" s="13">
         <v>0</v>
       </c>
       <c r="J51" s="15"/>
       <c r="K51" s="15"/>
     </row>
-    <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>67</v>
       </c>
       <c r="B52" s="11"/>
@@ -1523,19 +1467,19 @@
       <c r="F52" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="G52" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H52" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I52" s="13" t="n">
+      <c r="G52" s="13">
+        <v>0</v>
+      </c>
+      <c r="H52" s="13">
+        <v>0</v>
+      </c>
+      <c r="I52" s="13">
         <v>0</v>
       </c>
       <c r="J52" s="15"/>
       <c r="K52" s="15"/>
     </row>
-    <row r="54" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>59</v>
       </c>
@@ -1570,17 +1514,17 @@
         <v>66</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>95</v>
       </c>
       <c r="B55" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C55" s="12" t="n">
+      <c r="C55" s="12">
         <v>42076</v>
       </c>
-      <c r="D55" s="11" t="n">
+      <c r="D55" s="11">
         <v>55</v>
       </c>
       <c r="E55" s="11" t="s">
@@ -1589,7 +1533,7 @@
       <c r="F55" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="G55" s="14" t="n">
+      <c r="G55" s="14">
         <v>42082</v>
       </c>
       <c r="H55" s="13" t="s">
@@ -1605,24 +1549,24 @@
         <v>74</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>95</v>
       </c>
       <c r="B56" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C56" s="12" t="n">
+      <c r="C56" s="12">
         <v>42129</v>
       </c>
-      <c r="D56" s="11" t="n">
+      <c r="D56" s="11">
         <v>40</v>
       </c>
       <c r="E56" s="11"/>
       <c r="F56" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="G56" s="14" t="n">
+      <c r="G56" s="14">
         <v>42087</v>
       </c>
       <c r="H56" s="13" t="s">
@@ -1636,24 +1580,24 @@
       </c>
       <c r="K56" s="15"/>
     </row>
-    <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>95</v>
       </c>
       <c r="B57" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C57" s="12" t="n">
+      <c r="C57" s="12">
         <v>42151</v>
       </c>
-      <c r="D57" s="11" t="n">
+      <c r="D57" s="11">
         <v>60</v>
       </c>
       <c r="E57" s="11"/>
       <c r="F57" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="G57" s="14" t="n">
+      <c r="G57" s="14">
         <v>42159</v>
       </c>
       <c r="H57" s="13" t="s">
@@ -1667,8 +1611,8 @@
       </c>
       <c r="K57" s="15"/>
     </row>
-    <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>95</v>
       </c>
       <c r="B58" s="11" t="s">
@@ -1680,13 +1624,13 @@
       <c r="F58" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="G58" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H58" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I58" s="13" t="n">
+      <c r="G58" s="13">
+        <v>0</v>
+      </c>
+      <c r="H58" s="13">
+        <v>0</v>
+      </c>
+      <c r="I58" s="13">
         <v>0</v>
       </c>
       <c r="J58" s="15" t="s">
@@ -1694,8 +1638,8 @@
       </c>
       <c r="K58" s="15"/>
     </row>
-    <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>95</v>
       </c>
       <c r="B59" s="11"/>
@@ -1705,13 +1649,13 @@
       <c r="F59" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="G59" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H59" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I59" s="13" t="n">
+      <c r="G59" s="13">
+        <v>0</v>
+      </c>
+      <c r="H59" s="13">
+        <v>0</v>
+      </c>
+      <c r="I59" s="13">
         <v>0</v>
       </c>
       <c r="J59" s="15" t="s">
@@ -1719,8 +1663,8 @@
       </c>
       <c r="K59" s="15"/>
     </row>
-    <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>95</v>
       </c>
       <c r="B60" s="11"/>
@@ -1730,13 +1674,13 @@
       <c r="F60" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="G60" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H60" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I60" s="13" t="n">
+      <c r="G60" s="13">
+        <v>0</v>
+      </c>
+      <c r="H60" s="13">
+        <v>0</v>
+      </c>
+      <c r="I60" s="13">
         <v>0</v>
       </c>
       <c r="J60" s="15" t="s">
@@ -1744,8 +1688,8 @@
       </c>
       <c r="K60" s="15"/>
     </row>
-    <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>95</v>
       </c>
       <c r="B61" s="11"/>
@@ -1755,20 +1699,20 @@
       <c r="F61" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="G61" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H61" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I61" s="13" t="n">
+      <c r="G61" s="13">
+        <v>0</v>
+      </c>
+      <c r="H61" s="13">
+        <v>0</v>
+      </c>
+      <c r="I61" s="13">
         <v>0</v>
       </c>
       <c r="J61" s="15"/>
       <c r="K61" s="15"/>
     </row>
-    <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>95</v>
       </c>
       <c r="B62" s="11"/>
@@ -1778,7 +1722,7 @@
       <c r="F62" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="G62" s="14" t="n">
+      <c r="G62" s="14">
         <v>42110</v>
       </c>
       <c r="H62" s="13" t="s">
@@ -1790,8 +1734,8 @@
       <c r="J62" s="15"/>
       <c r="K62" s="15"/>
     </row>
-    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>95</v>
       </c>
       <c r="B63" s="11"/>
@@ -1801,7 +1745,7 @@
       <c r="F63" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="G63" s="14" t="n">
+      <c r="G63" s="14">
         <v>42128</v>
       </c>
       <c r="H63" s="13" t="s">
@@ -1813,7 +1757,7 @@
       <c r="J63" s="15"/>
       <c r="K63" s="15"/>
     </row>
-    <row r="65" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>59</v>
       </c>
@@ -1848,17 +1792,17 @@
         <v>66</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>101</v>
       </c>
       <c r="B66" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C66" s="12" t="n">
+      <c r="C66" s="12">
         <v>42076</v>
       </c>
-      <c r="D66" s="11" t="n">
+      <c r="D66" s="11">
         <v>55</v>
       </c>
       <c r="E66" s="11" t="s">
@@ -1867,7 +1811,7 @@
       <c r="F66" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="G66" s="14" t="n">
+      <c r="G66" s="14">
         <v>42082</v>
       </c>
       <c r="H66" s="13" t="s">
@@ -1879,28 +1823,28 @@
       <c r="J66" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="K66" s="15" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+      <c r="K66" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>101</v>
       </c>
       <c r="B67" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C67" s="12" t="n">
+      <c r="C67" s="12">
         <v>42129</v>
       </c>
-      <c r="D67" s="11" t="n">
+      <c r="D67" s="11">
         <v>40</v>
       </c>
       <c r="E67" s="11"/>
       <c r="F67" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="G67" s="14" t="n">
+      <c r="G67" s="14">
         <v>42087</v>
       </c>
       <c r="H67" s="13" t="s">
@@ -1914,24 +1858,24 @@
       </c>
       <c r="K67" s="15"/>
     </row>
-    <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>101</v>
       </c>
       <c r="B68" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C68" s="12" t="n">
+      <c r="C68" s="12">
         <v>42151</v>
       </c>
-      <c r="D68" s="11" t="n">
+      <c r="D68" s="11">
         <v>60</v>
       </c>
       <c r="E68" s="11"/>
       <c r="F68" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="G68" s="14" t="n">
+      <c r="G68" s="14">
         <v>42159</v>
       </c>
       <c r="H68" s="13" t="s">
@@ -1945,8 +1889,8 @@
       </c>
       <c r="K68" s="15"/>
     </row>
-    <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>101</v>
       </c>
       <c r="B69" s="11" t="s">
@@ -1958,13 +1902,13 @@
       <c r="F69" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="G69" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H69" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I69" s="13" t="n">
+      <c r="G69" s="13">
+        <v>0</v>
+      </c>
+      <c r="H69" s="13">
+        <v>0</v>
+      </c>
+      <c r="I69" s="13">
         <v>0</v>
       </c>
       <c r="J69" s="15" t="s">
@@ -1972,8 +1916,8 @@
       </c>
       <c r="K69" s="15"/>
     </row>
-    <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>101</v>
       </c>
       <c r="B70" s="11"/>
@@ -1983,7 +1927,7 @@
       <c r="F70" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="G70" s="14" t="n">
+      <c r="G70" s="14">
         <v>42128</v>
       </c>
       <c r="H70" s="13" t="s">
@@ -1997,8 +1941,8 @@
       </c>
       <c r="K70" s="15"/>
     </row>
-    <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>101</v>
       </c>
       <c r="B71" s="11"/>
@@ -2008,7 +1952,7 @@
       <c r="F71" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="G71" s="14" t="n">
+      <c r="G71" s="14">
         <v>42159</v>
       </c>
       <c r="H71" s="13" t="s">
@@ -2022,8 +1966,8 @@
       </c>
       <c r="K71" s="15"/>
     </row>
-    <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>101</v>
       </c>
       <c r="B72" s="11"/>
@@ -2034,19 +1978,19 @@
         <v>92</v>
       </c>
       <c r="G72" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H72" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="H72" s="13" t="s">
+      <c r="I72" s="13" t="s">
         <v>107</v>
-      </c>
-      <c r="I72" s="13" t="s">
-        <v>108</v>
       </c>
       <c r="J72" s="15"/>
       <c r="K72" s="15"/>
     </row>
-    <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>101</v>
       </c>
       <c r="B73" s="11"/>
@@ -2056,7 +2000,7 @@
       <c r="F73" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="G73" s="14" t="n">
+      <c r="G73" s="14">
         <v>42110</v>
       </c>
       <c r="H73" s="13" t="s">
@@ -2068,8 +2012,8 @@
       <c r="J73" s="15"/>
       <c r="K73" s="15"/>
     </row>
-    <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>101</v>
       </c>
       <c r="B74" s="11"/>
@@ -2079,7 +2023,7 @@
       <c r="F74" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="G74" s="14" t="n">
+      <c r="G74" s="14">
         <v>42128</v>
       </c>
       <c r="H74" s="13" t="s">
@@ -2092,58 +2036,33 @@
       <c r="K74" s="15"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix the date format
</commit_message>
<xml_diff>
--- a/data/management/Management_information_HAN_2015.xlsx
+++ b/data/management/Management_information_HAN_2015.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marse\seadrive_root\Tien-Che\My Libraries\PhD_Tien\Project\Briwecs\BRIWECS_Data_Publication\data\management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6942C6-ECD2-4621-86E2-ABE105CDF13D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89439E9D-4618-4303-B96D-AE546D9CB6F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="108">
   <si>
     <t>General information</t>
   </si>
@@ -351,9 +351,6 @@
   </si>
   <si>
     <t>Prosaro</t>
-  </si>
-  <si>
-    <t>16/06/2015</t>
   </si>
 </sst>
 </file>
@@ -572,9 +569,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in 20% - Accent3" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
@@ -844,7 +839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B56" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
@@ -1902,7 +1897,7 @@
       <c r="F69" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="G69" s="13">
+      <c r="G69" s="16">
         <v>0</v>
       </c>
       <c r="H69" s="13">
@@ -1977,8 +1972,8 @@
       <c r="F72" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="G72" s="16" t="s">
-        <v>108</v>
+      <c r="G72" s="14">
+        <v>42171</v>
       </c>
       <c r="H72" s="13" t="s">
         <v>106</v>
@@ -2037,7 +2032,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>